<commit_message>
Added Images + Spreadsheets
+ Finished Load process
+ Added images
+ Added spreadsheet for cleaned data
</commit_message>
<xml_diff>
--- a/dataset/customer_call_list.xlsx
+++ b/dataset/customer_call_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Pandas Tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjunsaini/Desktop/GithubRepos/Customer-List-ETL/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:40009_{E07D7DFE-C20E-4C0A-9299-C6166B0A5365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{890D025C-C355-436F-87C5-736415E1B8DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91A68BF-5983-6144-8BF1-4D8DCBF2D001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Call List" sheetId="1" r:id="rId1"/>
@@ -787,6 +787,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{21B8135B-D32F-3F4A-B037-2F524AE365D1}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22" xr:uid="{21B8135B-D32F-3F4A-B037-2F524AE365D1}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{7D1816E2-A637-CD4E-AE0D-04B58F06089B}" name="CustomerID"/>
+    <tableColumn id="2" xr3:uid="{3C5648AB-03C4-5C4E-BDF4-003260876A85}" name="First_Name"/>
+    <tableColumn id="3" xr3:uid="{0853E294-84E7-0646-B417-0DA29825D278}" name="Last_Name"/>
+    <tableColumn id="4" xr3:uid="{0C3CFB3A-7E02-9549-B8AD-4B25293B71AB}" name="Phone_Number"/>
+    <tableColumn id="5" xr3:uid="{E7126211-83B8-FA48-94A2-652BA3B5904A}" name="Address"/>
+    <tableColumn id="6" xr3:uid="{02AF98BA-4796-D142-9D90-62386299A245}" name="Paying Customer"/>
+    <tableColumn id="7" xr3:uid="{3EF4B737-6FD4-4042-AD12-D9C20BF4DC0E}" name="Do_Not_Contact"/>
+    <tableColumn id="8" xr3:uid="{AD587F1A-3B77-0B42-9304-7101C5925321}" name="Not_Useful_Column"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1088,25 +1105,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" customWidth="1"/>
+    <col min="6" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1159,7 +1175,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1186,7 +1202,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1210,7 +1226,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1237,7 +1253,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1264,7 +1280,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1291,7 +1307,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1315,7 +1331,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1342,7 +1358,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1363,7 +1379,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1390,7 +1406,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1414,7 +1430,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1438,7 +1454,7 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -1465,7 +1481,7 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -1492,7 +1508,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -1519,7 +1535,7 @@
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -1546,7 +1562,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -1573,7 +1589,7 @@
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1018</v>
       </c>
@@ -1597,7 +1613,7 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -1624,7 +1640,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1020</v>
       </c>
@@ -1651,7 +1667,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -1681,5 +1697,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>